<commit_message>
exchange: improve Import signatures and add log support
</commit_message>
<xml_diff>
--- a/exchange/nested_resource.xlsx
+++ b/exchange/nested_resource.xlsx
@@ -23,10 +23,10 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Address 01</t>
+    <t>Country 01</t>
   </si>
   <si>
-    <t>Address 02</t>
+    <t>Country 02</t>
   </si>
   <si>
     <t>Van</t>

</xml_diff>